<commit_message>
Add custom fields to load template
</commit_message>
<xml_diff>
--- a/khor/administration/plantilla_carga_expediente.xlsx
+++ b/khor/administration/plantilla_carga_expediente.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Expediente " sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">prueba_carga1@hotmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">miztli</t>
+    <t xml:space="preserve">miztli editado 2</t>
   </si>
   <si>
     <t xml:space="preserve">melgoza</t>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">del valle</t>
   </si>
   <si>
-    <t xml:space="preserve">no sé qué pedo</t>
+    <t xml:space="preserve">no sé</t>
   </si>
   <si>
     <t xml:space="preserve">menos</t>
@@ -95,10 +95,13 @@
     <t xml:space="preserve">recursos humanos</t>
   </si>
   <si>
-    <t xml:space="preserve">no sé</t>
-  </si>
-  <si>
     <t xml:space="preserve">25/01/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prueba_carga2@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citlalli 2</t>
   </si>
   <si>
     <t xml:space="preserve">fecha_ultima_evaluacion</t>
@@ -209,29 +212,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="21.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="17.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="10.72"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.7125506072875"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -313,22 +316,67 @@
         <v>23</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>34</v>
       </c>
       <c r="N2" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>25</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="prueba_carga1@hotmail.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="prueba_carga2@hotmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -343,16 +391,16 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.72"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7125506072875"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,19 +408,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Add requests for reports
</commit_message>
<xml_diff>
--- a/khor/administration/plantilla_carga_expediente.xlsx
+++ b/khor/administration/plantilla_carga_expediente.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Expediente " sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">prueba_carga1@hotmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">miztli editado 2</t>
+    <t xml:space="preserve">miztli</t>
   </si>
   <si>
     <t xml:space="preserve">melgoza</t>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">hernández</t>
   </si>
   <si>
-    <t xml:space="preserve">administrador</t>
+    <t xml:space="preserve">inexistente</t>
   </si>
   <si>
     <t xml:space="preserve">del valle</t>
@@ -101,7 +101,31 @@
     <t xml:space="preserve">prueba_carga2@hotmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Citlalli 2</t>
+    <t xml:space="preserve">citlalli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a prueba 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prueba_carga3@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leticia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a prueba 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcd1235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25/01/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prueba_carga4@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manuel</t>
   </si>
   <si>
     <t xml:space="preserve">fecha_ultima_evaluacion</t>
@@ -120,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -142,6 +166,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,12 +216,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -212,29 +246,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="18" min="16" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="10.7125506072875"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="21.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="17.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="10.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,7 +359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>25</v>
       </c>
@@ -341,11 +375,11 @@
       <c r="E3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>20</v>
@@ -369,14 +403,98 @@
         <v>24</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="prueba_carga1@hotmail.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="prueba_carga2@hotmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -391,16 +509,16 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7125506072875"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,19 +526,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>